<commit_message>
Changes for assignment 6.
</commit_message>
<xml_diff>
--- a/Assignment_6.xlsx
+++ b/Assignment_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SES\PSA\Assignments\Assignment6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CD41C2-8612-474E-B488-EC9ADC64063D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E57C5F-0796-4B9E-AA66-FDD07FBBD2C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5064" xr2:uid="{BC364D72-8EE9-47D8-A8C6-3483D0486FC5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>No. of elements</t>
   </si>
@@ -58,6 +58,27 @@
   </si>
   <si>
     <t>Mergesort with Instrumentation for no copy and with insurance</t>
+  </si>
+  <si>
+    <t>Quicksort Dual Pivot</t>
+  </si>
+  <si>
+    <t>Heapsort</t>
+  </si>
+  <si>
+    <t>Raw time across various sort algorithms (without instrumentation)</t>
+  </si>
+  <si>
+    <t>Hits comparison</t>
+  </si>
+  <si>
+    <t>Compares comparison</t>
+  </si>
+  <si>
+    <t>Raw time for Quicksort Dual Pivot (ms)</t>
+  </si>
+  <si>
+    <t>Raw time for Heap sort (ms)</t>
   </si>
 </sst>
 </file>
@@ -93,9 +114,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,7 +177,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>No. of elements Vs Time (ms)</a:t>
+              <a:t>Raw time across various sort algorithms</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -193,7 +222,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
+              <c:f>Sheet1!$B$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -228,7 +257,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$9</c:f>
+              <c:f>Sheet1!$A$54:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -255,7 +284,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$9</c:f>
+              <c:f>Sheet1!$B$54:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -283,7 +312,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3BB1-4F87-B746-2D35A68A860E}"/>
+              <c16:uniqueId val="{00000000-833A-4D6F-8458-47031A9AABEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -292,11 +321,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
+              <c:f>Sheet1!$C$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MS with insurance</c:v>
+                  <c:v>Quicksort Dual Pivot</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -327,7 +356,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$9</c:f>
+              <c:f>Sheet1!$A$54:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -354,27 +383,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$9</c:f>
+              <c:f>Sheet1!$C$54:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.51</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.37</c:v>
+                  <c:v>5.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.51</c:v>
+                  <c:v>11.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.93</c:v>
+                  <c:v>33.119999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.35</c:v>
+                  <c:v>67.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>156.62</c:v>
+                  <c:v>114.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -382,7 +411,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3BB1-4F87-B746-2D35A68A860E}"/>
+              <c16:uniqueId val="{00000001-833A-4D6F-8458-47031A9AABEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -391,11 +420,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
+              <c:f>Sheet1!$D$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MS with no copy</c:v>
+                  <c:v>Heapsort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -426,7 +455,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$9</c:f>
+              <c:f>Sheet1!$A$54:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -453,27 +482,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$9</c:f>
+              <c:f>Sheet1!$D$54:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>3.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.68</c:v>
+                  <c:v>7.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.67</c:v>
+                  <c:v>18.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.119999999999997</c:v>
+                  <c:v>56.74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.67</c:v>
+                  <c:v>98.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146.05000000000001</c:v>
+                  <c:v>234.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -481,106 +510,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3BB1-4F87-B746-2D35A68A860E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MS with no copy and with insurance</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$4:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>256000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$4:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.74</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>38.770000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>80.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>145.66999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3BB1-4F87-B746-2D35A68A860E}"/>
+              <c16:uniqueId val="{00000002-833A-4D6F-8458-47031A9AABEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -592,11 +522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="653647784"/>
-        <c:axId val="653653688"/>
+        <c:axId val="553111704"/>
+        <c:axId val="553115312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="653647784"/>
+        <c:axId val="553111704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,12 +638,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653653688"/>
+        <c:crossAx val="553115312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="653653688"/>
+        <c:axId val="553115312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,11 +684,24 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-IN"/>
-                  <a:t>Execution time(ms)</a:t>
+                  <a:t>Time</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0555555555555555E-2"/>
+              <c:y val="0.32744568387284917"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -825,7 +768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="653647784"/>
+        <c:crossAx val="553111704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -942,7 +885,7 @@
               <a:rPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Mergesort with Instrumentation</a:t>
+              <a:t>Hits comparison</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
@@ -984,25 +927,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$23</c:f>
+              <c:f>Sheet1!$B$67</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>No. of elements</c:v>
+                  <c:v>Merge Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1011,11 +954,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$24:$A$29</c:f>
+              <c:f>Sheet1!$A$68:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1039,11 +994,38 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$68:$B$73</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>440000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>960000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2080000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4480000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4800000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16211968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2EEB-4625-B35D-A70FE9515AB2}"/>
+              <c16:uniqueId val="{00000000-8C79-4612-A97A-C5D49FC7CE42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1052,17 +1034,17 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$23</c:f>
+              <c:f>Sheet1!$C$67</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Merge Sort</c:v>
+                  <c:v>Quicksort Dual Pivot</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1071,39 +1053,78 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$B$29</c:f>
+              <c:f>Sheet1!$A$68:$A$73</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.38</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.48</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>92.28</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>150.71</c:v>
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>256000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$68:$C$73</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>399059</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>863819</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1865195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4053554</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8595460</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14497699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2EEB-4625-B35D-A70FE9515AB2}"/>
+              <c16:uniqueId val="{00000001-8C79-4612-A97A-C5D49FC7CE42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1112,17 +1133,17 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$23</c:f>
+              <c:f>Sheet1!$D$67</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hits</c:v>
+                  <c:v>Heapsort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -1131,219 +1152,78 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$24:$C$29</c:f>
+              <c:f>Sheet1!$A$68:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>440000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>960000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2080000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4480000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4800000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16211968</c:v>
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>256000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2EEB-4625-B35D-A70FE9515AB2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Copies</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$24:$D$29</c:f>
+              <c:f>Sheet1!$D$68:$D$73</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>220000</c:v>
+                  <c:v>967573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>480000</c:v>
+                  <c:v>2095121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1040000</c:v>
+                  <c:v>4510171</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2240000</c:v>
+                  <c:v>9660304</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2400000</c:v>
+                  <c:v>20600980</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8105984</c:v>
+                  <c:v>34309291</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2EEB-4625-B35D-A70FE9515AB2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Swaps</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$24:$E$29</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9766</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19510</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>39020</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>78130</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>156192</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>224331</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-2EEB-4625-B35D-A70FE9515AB2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Compares</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$24:$F$29</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>121507</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>263005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>566000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1211998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2584026</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4303065</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-2EEB-4625-B35D-A70FE9515AB2}"/>
+              <c16:uniqueId val="{00000002-8C79-4612-A97A-C5D49FC7CE42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1355,18 +1235,86 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="697827328"/>
-        <c:axId val="697828968"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="697827328"/>
+        <c:axId val="594361624"/>
+        <c:axId val="594358344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="594361624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>No. of elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1375,8 +1323,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1403,15 +1351,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="697828968"/>
+        <c:crossAx val="594358344"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="697828968"/>
+        <c:axId val="594358344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,8 +1382,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1462,9 +1413,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="697827328"/>
+        <c:crossAx val="594361624"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1579,7 +1530,7 @@
               <a:rPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Mergesort with Instrumentation for no copy and with insurance</a:t>
+              <a:t>Compares comparison</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-IN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
@@ -1629,11 +1580,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$42</c:f>
+              <c:f>Sheet1!$B$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MS with no copy and with insurance</c:v>
+                  <c:v>Merge Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1664,7 +1615,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$43:$A$48</c:f>
+              <c:f>Sheet1!$A$82:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1691,27 +1642,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$B$48</c:f>
+              <c:f>Sheet1!$B$82:$B$87</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.12</c:v>
+                  <c:v>121507</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.35</c:v>
+                  <c:v>263005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.64</c:v>
+                  <c:v>566000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.43</c:v>
+                  <c:v>1211998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.81</c:v>
+                  <c:v>2584026</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>133.22999999999999</c:v>
+                  <c:v>4303065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1719,7 +1670,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AA66-4238-93EF-4861E8DEE9E0}"/>
+              <c16:uniqueId val="{00000000-FDD8-455E-B00E-FFA7CDCE2D91}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1728,11 +1679,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$42</c:f>
+              <c:f>Sheet1!$C$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hits</c:v>
+                  <c:v>Quicksort Dual Pivot</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1763,7 +1714,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$43:$A$48</c:f>
+              <c:f>Sheet1!$A$82:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1790,27 +1741,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$43:$C$48</c:f>
+              <c:f>Sheet1!$C$82:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>220000</c:v>
+                  <c:v>156251</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>619585</c:v>
+                  <c:v>339092</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1040000</c:v>
+                  <c:v>737757</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2240000</c:v>
+                  <c:v>1583346</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4800000</c:v>
+                  <c:v>3421208</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8105984</c:v>
+                  <c:v>5660545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,7 +1769,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AA66-4238-93EF-4861E8DEE9E0}"/>
+              <c16:uniqueId val="{00000001-FDD8-455E-B00E-FFA7CDCE2D91}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1827,11 +1778,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$42</c:f>
+              <c:f>Sheet1!$D$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Copies</c:v>
+                  <c:v>Heapsort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1862,7 +1813,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$43:$A$48</c:f>
+              <c:f>Sheet1!$A$82:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1889,27 +1840,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$43:$D$48</c:f>
+              <c:f>Sheet1!$D$82:$D$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>110000</c:v>
+                  <c:v>235372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260000</c:v>
+                  <c:v>510750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>520000</c:v>
+                  <c:v>1101490</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1120000</c:v>
+                  <c:v>2362973</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2400000</c:v>
+                  <c:v>5045946</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4052992</c:v>
+                  <c:v>8410537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1917,24 +1868,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-AA66-4238-93EF-4861E8DEE9E0}"/>
+              <c16:uniqueId val="{00000002-FDD8-455E-B00E-FFA7CDCE2D91}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Swaps</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1961,7 +1901,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$43:$A$48</c:f>
+              <c:f>Sheet1!$A$82:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1988,27 +1928,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$43:$E$48</c:f>
+              <c:f>Sheet1!$A$80</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9756</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19525</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39044</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>78055</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>156125</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>224278</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2016,106 +1941,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-AA66-4238-93EF-4861E8DEE9E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Compares</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$43:$A$48</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>160000</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>256000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$43:$F$48</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>123526</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>267062</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>574106</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1228247</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2616423</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4361167</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-AA66-4238-93EF-4861E8DEE9E0}"/>
+              <c16:uniqueId val="{00000004-FDD8-455E-B00E-FFA7CDCE2D91}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2127,11 +1953,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="727914720"/>
-        <c:axId val="727911768"/>
+        <c:axId val="611480168"/>
+        <c:axId val="611480496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="727914720"/>
+        <c:axId val="611480168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2151,6 +1977,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>No. of elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2188,12 +2069,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="727911768"/>
+        <c:crossAx val="611480496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="727911768"/>
+        <c:axId val="611480496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2094,37 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2250,7 +2161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="727914720"/>
+        <c:crossAx val="611480168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2967,7 +2878,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2994,8 +2905,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3075,11 +2986,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3090,11 +2996,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3106,7 +3007,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3126,9 +3027,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3141,10 +3039,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3184,22 +3082,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3304,8 +3203,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3437,19 +3336,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3463,6 +3363,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4002,23 +3913,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B1BD84-B244-4553-A180-DF385ECD4D40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774958B8-54BF-4CA1-B1C8-D362E40F5E47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4038,23 +3949,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D33DD4FA-5143-4DE6-A9CB-AEA781F4C9AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0F54A7-E0EC-4990-938E-2D61F309C4AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4074,23 +3985,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9646998B-8FA8-4FE1-9AB8-43E66280EFE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF112419-C480-45BD-8282-6E27F89A1F9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4408,429 +4319,1116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ADFFFD-6F13-4EBD-98DE-47434ECD2051}">
-  <dimension ref="A3:F48"/>
+  <dimension ref="A3:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>10000</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>3.58</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>3.51</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>20000</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>7.3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>7.37</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>6.68</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>6.74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>40000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>15.62</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>15.51</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>13.67</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>13.78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>80000</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>47.22</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>45.93</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>40.119999999999997</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>38.770000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>160000</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>89.67</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>88.35</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>79.67</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>80.42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>256000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>160.51</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>156.62</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>146.05000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>145.66999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>10000</v>
       </c>
-      <c r="B24">
+      <c r="B14" s="1">
         <v>3.38</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C14" s="2">
         <v>440000</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D14" s="2">
         <v>220000</v>
       </c>
-      <c r="E24" s="1">
-        <v>9766</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
         <v>121507</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>20000</v>
       </c>
-      <c r="B25">
+      <c r="B15" s="1">
         <v>3.4</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C15" s="2">
         <v>960000</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D15" s="2">
         <v>480000</v>
       </c>
-      <c r="E25" s="1">
-        <v>19510</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
         <v>263005</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>40000</v>
       </c>
-      <c r="B26">
+      <c r="B16" s="1">
         <v>15.48</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C16" s="2">
         <v>2080000</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D16" s="2">
         <v>1040000</v>
       </c>
-      <c r="E26">
-        <v>39020</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
         <v>566000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>80000</v>
       </c>
-      <c r="B27">
+      <c r="B17" s="1">
         <v>42.8</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C17" s="2">
         <v>4480000</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D17" s="2">
         <v>2240000</v>
       </c>
-      <c r="E27">
-        <v>78130</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
         <v>1211998</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>160000</v>
       </c>
-      <c r="B28">
+      <c r="B18" s="1">
         <v>92.28</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C18" s="2">
         <v>4800000</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D18" s="2">
         <v>2400000</v>
       </c>
-      <c r="E28">
-        <v>156192</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
         <v>2584026</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>256000</v>
       </c>
-      <c r="B29">
+      <c r="B19" s="1">
         <v>150.71</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C19" s="2">
         <v>16211968</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D19" s="2">
         <v>8105984</v>
       </c>
-      <c r="E29">
-        <v>224331</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
         <v>4303065</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>10000</v>
       </c>
-      <c r="B43">
+      <c r="B24" s="1">
         <v>3.12</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C24" s="2">
         <v>220000</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D24" s="2">
         <v>110000</v>
       </c>
-      <c r="E43" s="1">
-        <v>9756</v>
-      </c>
-      <c r="F43" s="1">
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
         <v>123526</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>20000</v>
       </c>
-      <c r="B44">
+      <c r="B25" s="1">
         <v>10.35</v>
       </c>
+      <c r="C25" s="2">
+        <v>619585</v>
+      </c>
+      <c r="D25" s="2">
+        <v>260000</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>267062</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B26" s="1">
+        <v>13.64</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1040000</v>
+      </c>
+      <c r="D26" s="2">
+        <v>520000</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>574106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B27" s="1">
+        <v>32.43</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2240000</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1120000</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1228247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B28" s="1">
+        <v>79.81</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4800000</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2400000</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2616423</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>256000</v>
+      </c>
+      <c r="B29" s="1">
+        <v>133.22999999999999</v>
+      </c>
+      <c r="C29" s="2">
+        <v>8105984</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4052992</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>4361167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B34" s="2">
+        <v>399059</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>61875</v>
+      </c>
+      <c r="E34" s="2">
+        <v>156251</v>
+      </c>
+      <c r="G34" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B35" s="2">
+        <v>863819</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>133396</v>
+      </c>
+      <c r="E35" s="2">
+        <v>339092</v>
+      </c>
+      <c r="G35" s="1">
+        <v>40000</v>
+      </c>
+      <c r="H35" s="1">
+        <v>11.46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1865195</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>285748</v>
+      </c>
+      <c r="E36" s="2">
+        <v>737757</v>
+      </c>
+      <c r="G36" s="1">
+        <v>80000</v>
+      </c>
+      <c r="H36" s="1">
+        <v>33.119999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4053554</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>626273</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1583346</v>
+      </c>
+      <c r="G37" s="1">
+        <v>160000</v>
+      </c>
+      <c r="H37" s="1">
+        <v>67.48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B38" s="2">
+        <v>8595460</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1308533</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3421208</v>
+      </c>
+      <c r="G38" s="1">
+        <v>256000</v>
+      </c>
+      <c r="H38" s="1">
+        <v>114.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>256000</v>
+      </c>
+      <c r="B39" s="2">
+        <v>14497699</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2237764</v>
+      </c>
+      <c r="E39" s="2">
+        <v>5660545</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H43" s="1">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B44" s="2">
+        <v>967573</v>
+      </c>
       <c r="C44" s="1">
-        <v>619585</v>
-      </c>
-      <c r="D44" s="1">
-        <v>260000</v>
-      </c>
-      <c r="E44" s="1">
-        <v>19525</v>
-      </c>
-      <c r="F44" s="1">
-        <v>267062</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>124207</v>
+      </c>
+      <c r="E44" s="2">
+        <v>235372</v>
+      </c>
+      <c r="G44" s="2">
+        <v>20000</v>
+      </c>
+      <c r="H44" s="1">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2095121</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
+        <v>268405</v>
+      </c>
+      <c r="E45" s="2">
+        <v>510750</v>
+      </c>
+      <c r="G45" s="1">
         <v>40000</v>
       </c>
-      <c r="B45">
-        <v>13.64</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1040000</v>
-      </c>
-      <c r="D45" s="1">
-        <v>520000</v>
-      </c>
-      <c r="E45" s="1">
-        <v>39044</v>
-      </c>
-      <c r="F45" s="1">
-        <v>574106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="H45" s="1">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B46" s="2">
+        <v>4510171</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>576798</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1101490</v>
+      </c>
+      <c r="G46" s="1">
         <v>80000</v>
       </c>
-      <c r="B46">
-        <v>32.43</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2240000</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1120000</v>
-      </c>
-      <c r="E46">
-        <v>78055</v>
-      </c>
-      <c r="F46" s="1">
-        <v>1228247</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="H46" s="1">
+        <v>56.74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B47" s="2">
+        <v>9660304</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1233589</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2362973</v>
+      </c>
+      <c r="G47" s="1">
         <v>160000</v>
       </c>
-      <c r="B47">
-        <v>79.81</v>
-      </c>
-      <c r="C47" s="1">
+      <c r="H47" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B48" s="2">
+        <v>20600980</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2627272</v>
+      </c>
+      <c r="E48" s="2">
+        <v>5045946</v>
+      </c>
+      <c r="G48" s="1">
+        <v>256000</v>
+      </c>
+      <c r="H48" s="1">
+        <v>234.81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>256000</v>
+      </c>
+      <c r="B49" s="2">
+        <v>34309291</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4372054</v>
+      </c>
+      <c r="E49" s="2">
+        <v>8410537</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B54" s="1">
+        <v>3.58</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2.54</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B55" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="C55" s="1">
+        <v>5.43</v>
+      </c>
+      <c r="D55" s="1">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B56" s="1">
+        <v>15.62</v>
+      </c>
+      <c r="C56" s="1">
+        <v>11.46</v>
+      </c>
+      <c r="D56" s="1">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B57" s="1">
+        <v>47.22</v>
+      </c>
+      <c r="C57" s="1">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="D57" s="1">
+        <v>56.74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B58" s="1">
+        <v>89.67</v>
+      </c>
+      <c r="C58" s="1">
+        <v>67.48</v>
+      </c>
+      <c r="D58" s="1">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>256000</v>
+      </c>
+      <c r="B59" s="1">
+        <v>160.51</v>
+      </c>
+      <c r="C59" s="1">
+        <v>114.5</v>
+      </c>
+      <c r="D59" s="1">
+        <v>234.81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B68" s="2">
+        <f>C14</f>
+        <v>440000</v>
+      </c>
+      <c r="C68" s="2">
+        <f>B34</f>
+        <v>399059</v>
+      </c>
+      <c r="D68" s="2">
+        <f>B44</f>
+        <v>967573</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B69" s="2">
+        <f t="shared" ref="B69:B73" si="0">C15</f>
+        <v>960000</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" ref="C69:C73" si="1">B35</f>
+        <v>863819</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" ref="D69:D73" si="2">B45</f>
+        <v>2095121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" si="0"/>
+        <v>2080000</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="1"/>
+        <v>1865195</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="2"/>
+        <v>4510171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B71" s="2">
+        <f t="shared" si="0"/>
+        <v>4480000</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="1"/>
+        <v>4053554</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="2"/>
+        <v>9660304</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B72" s="2">
+        <f t="shared" si="0"/>
         <v>4800000</v>
       </c>
-      <c r="D47" s="1">
-        <v>2400000</v>
-      </c>
-      <c r="E47" s="1">
-        <v>156125</v>
-      </c>
-      <c r="F47" s="1">
-        <v>2616423</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="C72" s="2">
+        <f t="shared" si="1"/>
+        <v>8595460</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="2"/>
+        <v>20600980</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
         <v>256000</v>
       </c>
-      <c r="B48">
-        <v>133.22999999999999</v>
-      </c>
-      <c r="C48" s="1">
-        <v>8105984</v>
-      </c>
-      <c r="D48" s="1">
-        <v>4052992</v>
-      </c>
-      <c r="E48">
-        <v>224278</v>
-      </c>
-      <c r="F48" s="1">
-        <v>4361167</v>
-      </c>
+      <c r="B73" s="2">
+        <f t="shared" si="0"/>
+        <v>16211968</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" si="1"/>
+        <v>14497699</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="2"/>
+        <v>34309291</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B82" s="2">
+        <f>F14</f>
+        <v>121507</v>
+      </c>
+      <c r="C82" s="2">
+        <f>E34</f>
+        <v>156251</v>
+      </c>
+      <c r="D82" s="2">
+        <f>E44</f>
+        <v>235372</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B83" s="2">
+        <f>F15</f>
+        <v>263005</v>
+      </c>
+      <c r="C83" s="2">
+        <f>E35</f>
+        <v>339092</v>
+      </c>
+      <c r="D83" s="2">
+        <f>E45</f>
+        <v>510750</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B84" s="2">
+        <f>F16</f>
+        <v>566000</v>
+      </c>
+      <c r="C84" s="2">
+        <f>E36</f>
+        <v>737757</v>
+      </c>
+      <c r="D84" s="2">
+        <f>E46</f>
+        <v>1101490</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B85" s="2">
+        <f>F17</f>
+        <v>1211998</v>
+      </c>
+      <c r="C85" s="2">
+        <f>E37</f>
+        <v>1583346</v>
+      </c>
+      <c r="D85" s="2">
+        <f>E47</f>
+        <v>2362973</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B86" s="2">
+        <f>F18</f>
+        <v>2584026</v>
+      </c>
+      <c r="C86" s="2">
+        <f>E38</f>
+        <v>3421208</v>
+      </c>
+      <c r="D86" s="2">
+        <f>E48</f>
+        <v>5045946</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>256000</v>
+      </c>
+      <c r="B87" s="2">
+        <f>F19</f>
+        <v>4303065</v>
+      </c>
+      <c r="C87" s="2">
+        <f>E39</f>
+        <v>5660545</v>
+      </c>
+      <c r="D87" s="2">
+        <f>E49</f>
+        <v>8410537</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>